<commit_message>
some code refactored, upgraded dependencies
</commit_message>
<xml_diff>
--- a/output/Khanty-Mansiysk/forecast.xlsx
+++ b/output/Khanty-Mansiysk/forecast.xlsx
@@ -412,7 +412,7 @@
   <cols>
     <col min="1" max="1" width="19.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="31.7109375" style="1" customWidth="1"/>
@@ -456,13 +456,13 @@
     </row>
     <row r="2" spans="1:10" ht="20" customHeight="1">
       <c r="A2" s="1">
-        <v>300</v>
+        <v>255</v>
       </c>
       <c r="B2" s="1">
-        <v>76657</v>
+        <v>9210</v>
       </c>
       <c r="C2" s="1">
-        <v>9210</v>
+        <v>30.70000076293945</v>
       </c>
       <c r="D2" s="1">
         <v>2000</v>
@@ -477,24 +477,24 @@
         <v>762</v>
       </c>
       <c r="H2" s="1">
+        <v>-23</v>
+      </c>
+      <c r="I2" s="1">
         <v>-56647</v>
       </c>
-      <c r="I2" s="1">
-        <v>-57179</v>
-      </c>
       <c r="J2" s="1">
-        <v>99</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20" customHeight="1">
       <c r="A3" s="1">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1">
-        <v>2868</v>
+        <v>646</v>
       </c>
       <c r="C3" s="1">
-        <v>646</v>
+        <v>14.04347801208496</v>
       </c>
       <c r="D3" s="1">
         <v>2001</v>
@@ -509,24 +509,24 @@
         <v>634</v>
       </c>
       <c r="H3" s="1">
+        <v>-41</v>
+      </c>
+      <c r="I3" s="1">
         <v>-89845</v>
       </c>
-      <c r="I3" s="1">
-        <v>-105741</v>
-      </c>
       <c r="J3" s="1">
-        <v>320</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="20" customHeight="1">
       <c r="A4" s="1">
-        <v>126</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1">
-        <v>6710</v>
+        <v>898</v>
       </c>
       <c r="C4" s="1">
-        <v>898</v>
+        <v>7.126984119415283</v>
       </c>
       <c r="D4" s="1">
         <v>2002</v>
@@ -541,24 +541,24 @@
         <v>633</v>
       </c>
       <c r="H4" s="1">
+        <v>35</v>
+      </c>
+      <c r="I4" s="1">
         <v>31251</v>
       </c>
-      <c r="I4" s="1">
-        <v>39994</v>
-      </c>
       <c r="J4" s="1">
-        <v>135</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="20" customHeight="1">
       <c r="A5" s="1">
-        <v>720</v>
+        <v>166</v>
       </c>
       <c r="B5" s="1">
-        <v>119922</v>
+        <v>9564</v>
       </c>
       <c r="C5" s="1">
-        <v>9564</v>
+        <v>13.28333377838135</v>
       </c>
       <c r="D5" s="1">
         <v>2003</v>
@@ -573,24 +573,24 @@
         <v>586</v>
       </c>
       <c r="H5" s="1">
+        <v>63</v>
+      </c>
+      <c r="I5" s="1">
         <v>19178</v>
       </c>
-      <c r="I5" s="1">
-        <v>56900</v>
-      </c>
       <c r="J5" s="1">
-        <v>571</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="20" customHeight="1">
       <c r="A6" s="1">
-        <v>959</v>
+        <v>288</v>
       </c>
       <c r="B6" s="1">
-        <v>276787</v>
+        <v>34271</v>
       </c>
       <c r="C6" s="1">
-        <v>34271</v>
+        <v>35.73618316650391</v>
       </c>
       <c r="D6" s="1">
         <v>2004</v>
@@ -605,24 +605,24 @@
         <v>415</v>
       </c>
       <c r="H6" s="1">
+        <v>158</v>
+      </c>
+      <c r="I6" s="1">
         <v>136886</v>
       </c>
-      <c r="I6" s="1">
-        <v>282543</v>
-      </c>
       <c r="J6" s="1">
-        <v>708</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="20" customHeight="1">
       <c r="A7" s="1">
-        <v>912</v>
+        <v>217</v>
       </c>
       <c r="B7" s="1">
-        <v>198551</v>
+        <v>58652</v>
       </c>
       <c r="C7" s="1">
-        <v>58652</v>
+        <v>64.3114013671875</v>
       </c>
       <c r="D7" s="1">
         <v>2005</v>
@@ -637,24 +637,24 @@
         <v>430</v>
       </c>
       <c r="H7" s="1">
+        <v>199</v>
+      </c>
+      <c r="I7" s="1">
         <v>196804</v>
       </c>
-      <c r="I7" s="1">
-        <v>377611</v>
-      </c>
       <c r="J7" s="1">
-        <v>759</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="20" customHeight="1">
       <c r="A8" s="1">
-        <v>453</v>
+        <v>131</v>
       </c>
       <c r="B8" s="1">
-        <v>59529</v>
+        <v>10614</v>
       </c>
       <c r="C8" s="1">
-        <v>10614</v>
+        <v>23.43046379089355</v>
       </c>
       <c r="D8" s="1">
         <v>2006</v>
@@ -669,24 +669,24 @@
         <v>465</v>
       </c>
       <c r="H8" s="1">
+        <v>54</v>
+      </c>
+      <c r="I8" s="1">
         <v>6904</v>
       </c>
-      <c r="I8" s="1">
-        <v>48306</v>
-      </c>
       <c r="J8" s="1">
-        <v>523</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="20" customHeight="1">
       <c r="A9" s="1">
-        <v>336</v>
+        <v>142</v>
       </c>
       <c r="B9" s="1">
-        <v>47835</v>
+        <v>26795</v>
       </c>
       <c r="C9" s="1">
-        <v>26795</v>
+        <v>79.74702453613281</v>
       </c>
       <c r="D9" s="1">
         <v>2007</v>
@@ -701,24 +701,24 @@
         <v>504</v>
       </c>
       <c r="H9" s="1">
+        <v>21</v>
+      </c>
+      <c r="I9" s="1">
         <v>-25653</v>
       </c>
-      <c r="I9" s="1">
-        <v>-11264</v>
-      </c>
       <c r="J9" s="1">
-        <v>444</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="20" customHeight="1">
       <c r="A10" s="1">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="B10" s="1">
-        <v>23477</v>
+        <v>5100</v>
       </c>
       <c r="C10" s="1">
-        <v>5100</v>
+        <v>21.51898765563965</v>
       </c>
       <c r="D10" s="1">
         <v>2008</v>
@@ -733,24 +733,24 @@
         <v>496</v>
       </c>
       <c r="H10" s="1">
+        <v>30</v>
+      </c>
+      <c r="I10" s="1">
         <v>-17228</v>
       </c>
-      <c r="I10" s="1">
-        <v>-8563</v>
-      </c>
       <c r="J10" s="1">
-        <v>424</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="20" customHeight="1">
       <c r="A11" s="1">
-        <v>529</v>
+        <v>131</v>
       </c>
       <c r="B11" s="1">
-        <v>69644</v>
+        <v>8732</v>
       </c>
       <c r="C11" s="1">
-        <v>8732</v>
+        <v>16.50661659240723</v>
       </c>
       <c r="D11" s="1">
         <v>2009</v>
@@ -765,24 +765,24 @@
         <v>455</v>
       </c>
       <c r="H11" s="1">
+        <v>62</v>
+      </c>
+      <c r="I11" s="1">
         <v>10476</v>
       </c>
-      <c r="I11" s="1">
-        <v>39825</v>
-      </c>
       <c r="J11" s="1">
-        <v>495</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="20" customHeight="1">
       <c r="A12" s="1">
-        <v>415</v>
+        <v>260</v>
       </c>
       <c r="B12" s="1">
-        <v>107979</v>
+        <v>61888</v>
       </c>
       <c r="C12" s="1">
-        <v>61888</v>
+        <v>149.1277160644531</v>
       </c>
       <c r="D12" s="1">
         <v>2010</v>
@@ -797,24 +797,24 @@
         <v>412</v>
       </c>
       <c r="H12" s="1">
+        <v>106</v>
+      </c>
+      <c r="I12" s="1">
         <v>47479</v>
       </c>
-      <c r="I12" s="1">
-        <v>80907</v>
-      </c>
       <c r="J12" s="1">
-        <v>517</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="20" customHeight="1">
       <c r="A13" s="1">
-        <v>825</v>
+        <v>228</v>
       </c>
       <c r="B13" s="1">
-        <v>188100</v>
+        <v>93465</v>
       </c>
       <c r="C13" s="1">
-        <v>93465</v>
+        <v>113.2909088134766</v>
       </c>
       <c r="D13" s="1">
         <v>2011</v>
@@ -829,24 +829,24 @@
         <v>355</v>
       </c>
       <c r="H13" s="1">
+        <v>190</v>
+      </c>
+      <c r="I13" s="1">
         <v>148930</v>
       </c>
-      <c r="I13" s="1">
-        <v>286757</v>
-      </c>
       <c r="J13" s="1">
-        <v>701</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="20" customHeight="1">
       <c r="A14" s="1">
-        <v>1235</v>
+        <v>1067</v>
       </c>
       <c r="B14" s="1">
-        <v>1317798</v>
+        <v>786198</v>
       </c>
       <c r="C14" s="1">
-        <v>786198</v>
+        <v>636.5975952148438</v>
       </c>
       <c r="D14" s="1">
         <v>2012</v>
@@ -861,24 +861,24 @@
         <v>330</v>
       </c>
       <c r="H14" s="1">
+        <v>573</v>
+      </c>
+      <c r="I14" s="1">
         <v>686201</v>
       </c>
-      <c r="I14" s="1">
-        <v>1163573</v>
-      </c>
       <c r="J14" s="1">
-        <v>1045</v>
+        <v>543</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="20" customHeight="1">
       <c r="A15" s="1">
-        <v>517</v>
+        <v>387</v>
       </c>
       <c r="B15" s="1">
-        <v>200479</v>
+        <v>134647</v>
       </c>
       <c r="C15" s="1">
-        <v>134647</v>
+        <v>260.4390563964844</v>
       </c>
       <c r="D15" s="1">
         <v>2013</v>
@@ -893,24 +893,24 @@
         <v>444</v>
       </c>
       <c r="H15" s="1">
+        <v>76</v>
+      </c>
+      <c r="I15" s="1">
         <v>29505</v>
       </c>
-      <c r="I15" s="1">
-        <v>87415</v>
-      </c>
       <c r="J15" s="1">
-        <v>561</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="20" customHeight="1">
       <c r="A16" s="1">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="B16" s="1">
-        <v>6074</v>
+        <v>1775</v>
       </c>
       <c r="C16" s="1">
-        <v>1775</v>
+        <v>18.88297843933105</v>
       </c>
       <c r="D16" s="1">
         <v>2014</v>
@@ -925,24 +925,24 @@
         <v>674</v>
       </c>
       <c r="H16" s="1">
+        <v>53</v>
+      </c>
+      <c r="I16" s="1">
         <v>66922</v>
       </c>
-      <c r="I16" s="1">
-        <v>96754</v>
-      </c>
       <c r="J16" s="1">
-        <v>64</v>
+        <v>-31</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="20" customHeight="1">
       <c r="A17" s="1">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="B17" s="1">
-        <v>10418</v>
+        <v>2338</v>
       </c>
       <c r="C17" s="1">
-        <v>2338</v>
+        <v>19.1639347076416</v>
       </c>
       <c r="D17" s="1">
         <v>2015</v>
@@ -957,24 +957,24 @@
         <v>833</v>
       </c>
       <c r="H17" s="1">
+        <v>43</v>
+      </c>
+      <c r="I17" s="1">
         <v>39391</v>
       </c>
-      <c r="I17" s="1">
-        <v>96187</v>
-      </c>
       <c r="J17" s="1">
-        <v>-46</v>
+        <v>-31</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="20" customHeight="1">
       <c r="A18" s="1">
-        <v>244</v>
+        <v>118</v>
       </c>
       <c r="B18" s="1">
-        <v>28917</v>
+        <v>18388</v>
       </c>
       <c r="C18" s="1">
-        <v>18388</v>
+        <v>75.36065673828125</v>
       </c>
       <c r="D18" s="1">
         <v>2016</v>
@@ -989,24 +989,24 @@
         <v>616</v>
       </c>
       <c r="H18" s="1">
+        <v>88</v>
+      </c>
+      <c r="I18" s="1">
         <v>39299</v>
       </c>
-      <c r="I18" s="1">
-        <v>66285</v>
-      </c>
       <c r="J18" s="1">
-        <v>577</v>
+        <v>334</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="20" customHeight="1">
       <c r="A19" s="1">
-        <v>383</v>
+        <v>259</v>
       </c>
       <c r="B19" s="1">
-        <v>99483</v>
+        <v>81724</v>
       </c>
       <c r="C19" s="1">
-        <v>81724</v>
+        <v>213.3785858154297</v>
       </c>
       <c r="D19" s="1">
         <v>2017</v>
@@ -1021,24 +1021,24 @@
         <v>428</v>
       </c>
       <c r="H19" s="1">
+        <v>104</v>
+      </c>
+      <c r="I19" s="1">
         <v>64934</v>
       </c>
-      <c r="I19" s="1">
-        <v>154783</v>
-      </c>
       <c r="J19" s="1">
-        <v>621</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="20" customHeight="1">
       <c r="A20" s="1">
-        <v>558</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1">
-        <v>24722</v>
+        <v>12674</v>
       </c>
       <c r="C20" s="1">
-        <v>12674</v>
+        <v>22.7132625579834</v>
       </c>
       <c r="D20" s="1">
         <v>2018</v>
@@ -1053,24 +1053,24 @@
         <v>499</v>
       </c>
       <c r="H20" s="1">
+        <v>46</v>
+      </c>
+      <c r="I20" s="1">
         <v>1597</v>
       </c>
-      <c r="I20" s="1">
-        <v>-3711</v>
-      </c>
       <c r="J20" s="1">
-        <v>361</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="20" customHeight="1">
       <c r="A21" s="1">
-        <v>543</v>
+        <v>57</v>
       </c>
       <c r="B21" s="1">
-        <v>31199</v>
+        <v>9198</v>
       </c>
       <c r="C21" s="1">
-        <v>9198</v>
+        <v>16.9392261505127</v>
       </c>
       <c r="D21" s="1">
         <v>2019</v>
@@ -1085,24 +1085,24 @@
         <v>469</v>
       </c>
       <c r="H21" s="1">
+        <v>60</v>
+      </c>
+      <c r="I21" s="1">
         <v>17716</v>
       </c>
-      <c r="I21" s="1">
-        <v>76254</v>
-      </c>
       <c r="J21" s="1">
-        <v>562</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="20" customHeight="1">
       <c r="A22" s="1">
-        <v>633</v>
+        <v>339</v>
       </c>
       <c r="B22" s="1">
-        <v>227985</v>
+        <v>185155</v>
       </c>
       <c r="C22" s="1">
-        <v>185155</v>
+        <v>261.9937133789062</v>
       </c>
       <c r="D22" s="1">
         <v>2020</v>
@@ -1117,13 +1117,13 @@
         <v>485</v>
       </c>
       <c r="H22" s="1">
+        <v>198</v>
+      </c>
+      <c r="I22" s="1">
         <v>197834</v>
       </c>
-      <c r="I22" s="1">
-        <v>357497</v>
-      </c>
       <c r="J22" s="1">
-        <v>747</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>